<commit_message>
Added Booking info (booking ID) to the Report.  Refactored release info.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28120" yWindow="6340" windowWidth="27660" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="-27480" yWindow="7160" windowWidth="27660" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CustodyStatusChangeReport" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>Race</t>
   </si>
@@ -78,15 +78,9 @@
     <t>Person last name</t>
   </si>
   <si>
-    <t>changed to finger print number</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
-    <t>Detention</t>
-  </si>
-  <si>
     <t>Sample Data</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>Facility ID</t>
   </si>
   <si>
-    <t>ID of the detention facility.</t>
-  </si>
-  <si>
     <t>Custody Release Date/Time</t>
   </si>
   <si>
@@ -189,12 +180,6 @@
     <t>Zip Code</t>
   </si>
   <si>
-    <t>Facility Name</t>
-  </si>
-  <si>
-    <t>Name of the detention facility</t>
-  </si>
-  <si>
     <t>/crr-doc:CustodyReleaseReport/nc:DocumentCreationDate/nc:DateTime</t>
   </si>
   <si>
@@ -213,83 +198,105 @@
     <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Case/nc:CaseDocketID</t>
   </si>
   <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/j:PersonEthnicityCode</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/j:PersonRaceCode</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/nc:PersonSSNIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationSourceText</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:PersonFBIIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/j:PersonSexCode</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleasePerson/@structures:ref]/nc:PersonPrimaryLanguage/nc:LanguageName</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionFacility/nc:FacilityName</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ActivityDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ActivityDescriptionText</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ActivityReasonText</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:AddressSecondaryUnitText</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/j:LocationStateNCICLISCode</t>
-  </si>
-  <si>
-    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Detention/nc:SupervisionRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
-  </si>
-  <si>
     <t>Document</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>Booking number</t>
+  </si>
+  <si>
+    <t>An assigned identification that identifies a subject at booking.</t>
+  </si>
+  <si>
+    <t>Booking Date/Time</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/j:PersonEthnicityCode</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/j:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/nc:PersonSSNIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseCardIdentification/nc:IdentificationSourceText</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/j:PersonAugmentation/j:PersonFBIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/nc:PersonPrimaryLanguage/nc:LanguageName</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/j:LocationStateNCICLISCode</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Location[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleaseToLocation/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingFacility/nc:FacilityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ActivityReasonText</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -323,13 +330,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,6 +351,26 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -385,727 +405,727 @@
   </borders>
   <cellStyleXfs count="715">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1129,26 +1149,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1156,8 +1161,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="715">
@@ -2204,11 +2243,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L356"/>
+  <dimension ref="A1:E357"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2217,11 +2256,11 @@
     <col min="2" max="2" width="25.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="88" style="1" customWidth="1"/>
+    <col min="5" max="5" width="104.83203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2232,22 +2271,22 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A2" s="19" t="s">
-        <v>87</v>
+    <row r="2" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A2" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:12" s="11" customFormat="1" ht="28">
+    <row r="3" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -2257,10 +2296,10 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="11" customFormat="1" ht="14">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="10" customFormat="1" ht="14">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2270,243 +2309,216 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A5" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12" t="s">
+    </row>
+    <row r="6" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12" t="s">
+      <c r="E6" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A8" s="19" t="s">
-        <v>35</v>
+      <c r="E7" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A8" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" s="11" customFormat="1" ht="14">
+    </row>
+    <row r="9" spans="1:5" s="10" customFormat="1" ht="14">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" spans="1:12" s="11" customFormat="1" ht="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="10" customFormat="1" ht="14">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A11" s="19" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A11" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:12" s="11" customFormat="1" ht="28">
+    <row r="12" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="11" customFormat="1" ht="28">
+    <row r="13" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="11" customFormat="1" ht="28">
+    <row r="14" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="15" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="16" spans="1:5" s="10" customFormat="1" ht="42">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="11" customFormat="1" ht="42">
+    </row>
+    <row r="17" spans="1:5" s="10" customFormat="1" ht="42">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="18" spans="1:5" s="10" customFormat="1" ht="42">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="19" spans="1:5" s="10" customFormat="1" ht="42">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="20" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="21" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A21" s="5"/>
       <c r="B21" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="22" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>18</v>
@@ -2516,210 +2528,210 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="11" customFormat="1" ht="28">
+    <row r="23" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A23" s="9"/>
       <c r="B23" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="11" customFormat="1" ht="42">
+    <row r="24" spans="1:5" s="10" customFormat="1" ht="28">
       <c r="A24" s="9"/>
       <c r="B24" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="8"/>
       <c r="E24" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-    </row>
-    <row r="25" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A25" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" s="11" customFormat="1" ht="28">
-      <c r="A26" s="12"/>
-      <c r="B26" s="9" t="s">
+    </row>
+    <row r="25" spans="1:5" s="17" customFormat="1">
+      <c r="A25" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" s="18" customFormat="1" ht="28">
+      <c r="B26" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="17" customFormat="1">
+      <c r="A27" s="21"/>
+      <c r="B27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="17" customFormat="1">
+      <c r="A28" s="21"/>
+      <c r="B28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="13" customFormat="1" ht="14">
+      <c r="A29" s="12"/>
+      <c r="B29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="13" customFormat="1" ht="28">
+      <c r="A30" s="7"/>
+      <c r="B30" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C30" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E30" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="10" customFormat="1" ht="14" hidden="1">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A33" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" s="10" customFormat="1" ht="28">
+      <c r="A34" s="11"/>
+      <c r="B34" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A27" s="12"/>
-      <c r="B27" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="10" t="s">
+    <row r="35" spans="1:5" s="13" customFormat="1" ht="28">
+      <c r="A35" s="12"/>
+      <c r="B35" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="18" customFormat="1" ht="14">
-      <c r="A28" s="17"/>
-      <c r="B28" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="18" t="s">
+    <row r="36" spans="1:5" s="13" customFormat="1" ht="28">
+      <c r="A36" s="7"/>
+      <c r="B36" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="18" customFormat="1" ht="28">
-      <c r="A29" s="7"/>
-      <c r="B29" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="7" t="s">
+    <row r="37" spans="1:5" s="10" customFormat="1" ht="28">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12" t="s">
+    <row r="38" spans="1:5" s="10" customFormat="1" ht="28">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="11" customFormat="1" ht="14" hidden="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:12" s="11" customFormat="1" ht="14">
-      <c r="A32" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" s="11" customFormat="1" ht="42">
-      <c r="A33" s="12"/>
-      <c r="B33" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="18" customFormat="1" ht="42">
-      <c r="A34" s="17"/>
-      <c r="B34" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="18" customFormat="1" ht="42">
-      <c r="A35" s="7"/>
-      <c r="B35" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="11" customFormat="1" ht="42">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="11" customFormat="1" ht="42">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="11" customFormat="1" ht="14">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="1:5" s="11" customFormat="1" ht="14">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" spans="1:5" s="11" customFormat="1" ht="14">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="1:5" s="11" customFormat="1" ht="14">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42" spans="1:5" s="11" customFormat="1" ht="14">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+    <row r="39" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="1:5" s="10" customFormat="1" ht="14">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="6"/>
@@ -4128,7 +4140,7 @@
       <c r="D244" s="6"/>
       <c r="E244" s="6"/>
     </row>
-    <row r="245" spans="1:5" hidden="1">
+    <row r="245" spans="1:5">
       <c r="A245" s="6"/>
       <c r="B245" s="6"/>
       <c r="C245" s="6"/>
@@ -4226,7 +4238,7 @@
       <c r="D258" s="6"/>
       <c r="E258" s="6"/>
     </row>
-    <row r="259" spans="1:5">
+    <row r="259" spans="1:5" hidden="1">
       <c r="A259" s="6"/>
       <c r="B259" s="6"/>
       <c r="C259" s="6"/>
@@ -4911,6 +4923,13 @@
       <c r="C356" s="6"/>
       <c r="D356" s="6"/>
       <c r="E356" s="6"/>
+    </row>
+    <row r="357" spans="1:5">
+      <c r="A357" s="6"/>
+      <c r="B357" s="6"/>
+      <c r="C357" s="6"/>
+      <c r="D357" s="6"/>
+      <c r="E357" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A8:J35">

</xml_diff>

<commit_message>
Updated Booking, Custody Release and Custody Status Reporting SSPs to carry the person health information exchange information.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Custody_Release_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27480" yWindow="7160" windowWidth="27660" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="-26900" yWindow="7380" windowWidth="27680" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="CustodyStatusChangeReport" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
   <si>
     <t>Race</t>
   </si>
@@ -283,13 +283,65 @@
   </si>
   <si>
     <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ActivityReasonText</t>
+  </si>
+  <si>
+    <t>Unique and Timeless ID</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Will be used only for record matching and will not be included in analytics data store</t>
+  </si>
+  <si>
+    <t>Behavioral Health</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>SMI Indicator</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Person[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/j:Booking/j:BookingRelease/nc:ReleasePerson/@structures:ref]/crr-ext:PersonPersistentIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Identity[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:PersonAliasIdentityAssociation[nc:Person/@structures:ref=/crr-doc:CustodyReleaseReport/crr-ext:Custody//nc:Person/@structures:id]/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Identity[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:PersonAliasIdentityAssociation[nc:Person/@structures:ref=/crr-doc:CustodyReleaseReport/crr-ext:Custody//nc:Person/@structures:id]/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Identity[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:PersonAliasIdentityAssociation[nc:Person/@structures:ref=/crr-doc:CustodyReleaseReport/crr-ext:Custody//nc:Person/@structures:id]/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Identity[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:PersonAliasIdentityAssociation[nc:Person/@structures:ref=/crr-doc:CustodyReleaseReport/crr-ext:Custody//nc:Person/@structures:id]/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:Identity[@structures:id=/crr-doc:CustodyReleaseReport/crr-ext:Custody/nc:PersonAliasIdentityAssociation[nc:Person/@structures:ref=/crr-doc:CustodyReleaseReport/crr-ext:Custody//nc:Person/@structures:id]/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation/j:Evaluation/j:EvaluationDiagnosisDescriptionText</t>
+  </si>
+  <si>
+    <t>crr-doc:CustodyReleaseReport/crr-ext:Custody/crr-ext:BehavioralHealthInformation/crr-ext:SeriousMentalIllnessIndicator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -373,6 +425,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -394,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -402,769 +460,831 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="715">
+  <cellStyleXfs count="725">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1173,33 +1293,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="715">
+  <cellStyles count="725">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1557,6 +1670,11 @@
     <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1914,6 +2032,11 @@
     <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2243,11 +2366,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E357"/>
+  <dimension ref="A1:L368"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="A48:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2260,7 +2383,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2277,7 +2400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
@@ -2286,7 +2409,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" s="10" customFormat="1" ht="28">
+    <row r="3" spans="1:12" s="10" customFormat="1" ht="28">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -2299,7 +2422,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="4" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -2312,7 +2435,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="5" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +2444,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="6" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A6" s="11"/>
       <c r="B6" s="11" t="s">
         <v>14</v>
@@ -2333,7 +2456,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="7" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
         <v>16</v>
@@ -2345,7 +2468,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="8" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
@@ -2354,7 +2477,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="9" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
         <v>39</v>
@@ -2365,7 +2488,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="10" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
         <v>40</v>
@@ -2376,7 +2499,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="11" spans="1:12" s="10" customFormat="1" ht="14">
       <c r="A11" s="14" t="s">
         <v>19</v>
       </c>
@@ -2385,495 +2508,652 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:12" s="33" customFormat="1" ht="45">
+      <c r="A12" s="31"/>
+      <c r="B12" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+    </row>
+    <row r="13" spans="1:12" s="28" customFormat="1" ht="14">
+      <c r="A13" s="27"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="s">
+    <row r="15" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
+    <row r="16" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="4" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="10" customFormat="1" ht="42">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="10" customFormat="1" ht="42">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" ht="42">
+    <row r="18" spans="1:12" s="10" customFormat="1" ht="42">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="10" customFormat="1" ht="42">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="10" customFormat="1" ht="42">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>28</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="10" customFormat="1" ht="42">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A21" s="5"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="10" customFormat="1" ht="42">
+      <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="10" customFormat="1" ht="28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="10" customFormat="1" ht="28">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A23" s="9"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A23" s="5"/>
       <c r="B23" s="9" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9" t="s">
+    <row r="26" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="4" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="17" customFormat="1">
-      <c r="A25" s="15" t="s">
+    <row r="27" spans="1:12" s="30" customFormat="1">
+      <c r="A27" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+    </row>
+    <row r="28" spans="1:12" s="35" customFormat="1" ht="60">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="35" customFormat="1" ht="70" customHeight="1">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="L29" s="35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="35" customFormat="1" ht="74" customHeight="1">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="L30" s="35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="35" customFormat="1" ht="72" customHeight="1">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="35" customFormat="1" ht="45">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="17" customFormat="1">
+      <c r="A33" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="1:5" s="18" customFormat="1" ht="28">
-      <c r="B26" s="25" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="1:12" s="18" customFormat="1" ht="28">
+      <c r="B34" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C34" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20" t="s">
+      <c r="D34" s="19"/>
+      <c r="E34" s="20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="17" customFormat="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="7" t="s">
+    <row r="35" spans="1:12" s="17" customFormat="1">
+      <c r="A35" s="21"/>
+      <c r="B35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23" t="s">
+      <c r="D35" s="22"/>
+      <c r="E35" s="23" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="17" customFormat="1">
-      <c r="A28" s="21"/>
-      <c r="B28" s="7" t="s">
+    <row r="36" spans="1:12" s="17" customFormat="1">
+      <c r="A36" s="21"/>
+      <c r="B36" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24" t="s">
+      <c r="D36" s="23"/>
+      <c r="E36" s="24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="13" customFormat="1" ht="14">
-      <c r="A29" s="12"/>
-      <c r="B29" s="9" t="s">
+    <row r="37" spans="1:12" s="13" customFormat="1" ht="14">
+      <c r="A37" s="12"/>
+      <c r="B37" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E37" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="13" customFormat="1" ht="28">
-      <c r="A30" s="7"/>
-      <c r="B30" s="13" t="s">
+    <row r="38" spans="1:12" s="13" customFormat="1" ht="28">
+      <c r="A38" s="7"/>
+      <c r="B38" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C38" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="10" customFormat="1" ht="14">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11" t="s">
+    <row r="39" spans="1:12" s="10" customFormat="1" ht="14">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C39" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11" t="s">
+      <c r="D39" s="11"/>
+      <c r="E39" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="10" customFormat="1" ht="14" hidden="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="1:5" s="10" customFormat="1" ht="14">
-      <c r="A33" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A34" s="11"/>
-      <c r="B34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="13" customFormat="1" ht="28">
-      <c r="A35" s="12"/>
-      <c r="B35" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="13" customFormat="1" ht="28">
-      <c r="A36" s="7"/>
-      <c r="B36" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="10" customFormat="1" ht="28">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="10" customFormat="1" ht="14">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-    </row>
-    <row r="40" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="40" spans="1:12" s="10" customFormat="1" ht="14" hidden="1">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
     </row>
-    <row r="41" spans="1:5" s="10" customFormat="1" ht="14">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="1:5" s="10" customFormat="1" ht="14">
+    <row r="41" spans="1:12" s="10" customFormat="1" ht="14">
+      <c r="A41" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" s="10" customFormat="1" ht="28">
       <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="1:5" s="10" customFormat="1" ht="14">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="B42" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="13" customFormat="1" ht="28">
+      <c r="A43" s="12"/>
+      <c r="B43" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="13" customFormat="1" ht="28">
+      <c r="A44" s="7"/>
+      <c r="B44" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="10" customFormat="1" ht="28">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="30" customFormat="1">
+      <c r="A47" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+    </row>
+    <row r="48" spans="1:12" s="35" customFormat="1" ht="30">
+      <c r="A48" s="36"/>
+      <c r="B48" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+    </row>
+    <row r="49" spans="1:8" s="35" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A49" s="36"/>
+      <c r="B49" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" s="32"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+    </row>
+    <row r="50" spans="1:8" s="10" customFormat="1" ht="14">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+    </row>
+    <row r="51" spans="1:8" s="10" customFormat="1" ht="14">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+    </row>
+    <row r="52" spans="1:8" s="10" customFormat="1" ht="14">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="1:8" s="10" customFormat="1" ht="14">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="1:8" s="10" customFormat="1" ht="14">
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:8">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:8">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:8">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:8">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:8">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:8">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:8">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:8">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:8">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -4147,77 +4427,77 @@
       <c r="D245" s="6"/>
       <c r="E245" s="6"/>
     </row>
-    <row r="246" spans="1:5" hidden="1">
+    <row r="246" spans="1:5">
       <c r="A246" s="6"/>
       <c r="B246" s="6"/>
       <c r="C246" s="6"/>
       <c r="D246" s="6"/>
       <c r="E246" s="6"/>
     </row>
-    <row r="247" spans="1:5" hidden="1">
+    <row r="247" spans="1:5">
       <c r="A247" s="6"/>
       <c r="B247" s="6"/>
       <c r="C247" s="6"/>
       <c r="D247" s="6"/>
       <c r="E247" s="6"/>
     </row>
-    <row r="248" spans="1:5" hidden="1">
+    <row r="248" spans="1:5">
       <c r="A248" s="6"/>
       <c r="B248" s="6"/>
       <c r="C248" s="6"/>
       <c r="D248" s="6"/>
       <c r="E248" s="6"/>
     </row>
-    <row r="249" spans="1:5" hidden="1">
+    <row r="249" spans="1:5">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="C249" s="6"/>
       <c r="D249" s="6"/>
       <c r="E249" s="6"/>
     </row>
-    <row r="250" spans="1:5" hidden="1">
+    <row r="250" spans="1:5">
       <c r="A250" s="6"/>
       <c r="B250" s="6"/>
       <c r="C250" s="6"/>
       <c r="D250" s="6"/>
       <c r="E250" s="6"/>
     </row>
-    <row r="251" spans="1:5" hidden="1">
+    <row r="251" spans="1:5">
       <c r="A251" s="6"/>
       <c r="B251" s="6"/>
       <c r="C251" s="6"/>
       <c r="D251" s="6"/>
       <c r="E251" s="6"/>
     </row>
-    <row r="252" spans="1:5" hidden="1">
+    <row r="252" spans="1:5">
       <c r="A252" s="6"/>
       <c r="B252" s="6"/>
       <c r="C252" s="6"/>
       <c r="D252" s="6"/>
       <c r="E252" s="6"/>
     </row>
-    <row r="253" spans="1:5" hidden="1">
+    <row r="253" spans="1:5">
       <c r="A253" s="6"/>
       <c r="B253" s="6"/>
       <c r="C253" s="6"/>
       <c r="D253" s="6"/>
       <c r="E253" s="6"/>
     </row>
-    <row r="254" spans="1:5" hidden="1">
+    <row r="254" spans="1:5">
       <c r="A254" s="6"/>
       <c r="B254" s="6"/>
       <c r="C254" s="6"/>
       <c r="D254" s="6"/>
       <c r="E254" s="6"/>
     </row>
-    <row r="255" spans="1:5" hidden="1">
+    <row r="255" spans="1:5">
       <c r="A255" s="6"/>
       <c r="B255" s="6"/>
       <c r="C255" s="6"/>
       <c r="D255" s="6"/>
       <c r="E255" s="6"/>
     </row>
-    <row r="256" spans="1:5" hidden="1">
+    <row r="256" spans="1:5">
       <c r="A256" s="6"/>
       <c r="B256" s="6"/>
       <c r="C256" s="6"/>
@@ -4245,77 +4525,77 @@
       <c r="D259" s="6"/>
       <c r="E259" s="6"/>
     </row>
-    <row r="260" spans="1:5">
+    <row r="260" spans="1:5" hidden="1">
       <c r="A260" s="6"/>
       <c r="B260" s="6"/>
       <c r="C260" s="6"/>
       <c r="D260" s="6"/>
       <c r="E260" s="6"/>
     </row>
-    <row r="261" spans="1:5">
+    <row r="261" spans="1:5" hidden="1">
       <c r="A261" s="6"/>
       <c r="B261" s="6"/>
       <c r="C261" s="6"/>
       <c r="D261" s="6"/>
       <c r="E261" s="6"/>
     </row>
-    <row r="262" spans="1:5">
+    <row r="262" spans="1:5" hidden="1">
       <c r="A262" s="6"/>
       <c r="B262" s="6"/>
       <c r="C262" s="6"/>
       <c r="D262" s="6"/>
       <c r="E262" s="6"/>
     </row>
-    <row r="263" spans="1:5">
+    <row r="263" spans="1:5" hidden="1">
       <c r="A263" s="6"/>
       <c r="B263" s="6"/>
       <c r="C263" s="6"/>
       <c r="D263" s="6"/>
       <c r="E263" s="6"/>
     </row>
-    <row r="264" spans="1:5">
+    <row r="264" spans="1:5" hidden="1">
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="C264" s="6"/>
       <c r="D264" s="6"/>
       <c r="E264" s="6"/>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:5" hidden="1">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="C265" s="6"/>
       <c r="D265" s="6"/>
       <c r="E265" s="6"/>
     </row>
-    <row r="266" spans="1:5">
+    <row r="266" spans="1:5" hidden="1">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="C266" s="6"/>
       <c r="D266" s="6"/>
       <c r="E266" s="6"/>
     </row>
-    <row r="267" spans="1:5">
+    <row r="267" spans="1:5" hidden="1">
       <c r="A267" s="6"/>
       <c r="B267" s="6"/>
       <c r="C267" s="6"/>
       <c r="D267" s="6"/>
       <c r="E267" s="6"/>
     </row>
-    <row r="268" spans="1:5">
+    <row r="268" spans="1:5" hidden="1">
       <c r="A268" s="6"/>
       <c r="B268" s="6"/>
       <c r="C268" s="6"/>
       <c r="D268" s="6"/>
       <c r="E268" s="6"/>
     </row>
-    <row r="269" spans="1:5">
+    <row r="269" spans="1:5" hidden="1">
       <c r="A269" s="6"/>
       <c r="B269" s="6"/>
       <c r="C269" s="6"/>
       <c r="D269" s="6"/>
       <c r="E269" s="6"/>
     </row>
-    <row r="270" spans="1:5">
+    <row r="270" spans="1:5" hidden="1">
       <c r="A270" s="6"/>
       <c r="B270" s="6"/>
       <c r="C270" s="6"/>
@@ -4931,11 +5211,88 @@
       <c r="D357" s="6"/>
       <c r="E357" s="6"/>
     </row>
+    <row r="358" spans="1:5">
+      <c r="A358" s="6"/>
+      <c r="B358" s="6"/>
+      <c r="C358" s="6"/>
+      <c r="D358" s="6"/>
+      <c r="E358" s="6"/>
+    </row>
+    <row r="359" spans="1:5">
+      <c r="A359" s="6"/>
+      <c r="B359" s="6"/>
+      <c r="C359" s="6"/>
+      <c r="D359" s="6"/>
+      <c r="E359" s="6"/>
+    </row>
+    <row r="360" spans="1:5">
+      <c r="A360" s="6"/>
+      <c r="B360" s="6"/>
+      <c r="C360" s="6"/>
+      <c r="D360" s="6"/>
+      <c r="E360" s="6"/>
+    </row>
+    <row r="361" spans="1:5">
+      <c r="A361" s="6"/>
+      <c r="B361" s="6"/>
+      <c r="C361" s="6"/>
+      <c r="D361" s="6"/>
+      <c r="E361" s="6"/>
+    </row>
+    <row r="362" spans="1:5">
+      <c r="A362" s="6"/>
+      <c r="B362" s="6"/>
+      <c r="C362" s="6"/>
+      <c r="D362" s="6"/>
+      <c r="E362" s="6"/>
+    </row>
+    <row r="363" spans="1:5">
+      <c r="A363" s="6"/>
+      <c r="B363" s="6"/>
+      <c r="C363" s="6"/>
+      <c r="D363" s="6"/>
+      <c r="E363" s="6"/>
+    </row>
+    <row r="364" spans="1:5">
+      <c r="A364" s="6"/>
+      <c r="B364" s="6"/>
+      <c r="C364" s="6"/>
+      <c r="D364" s="6"/>
+      <c r="E364" s="6"/>
+    </row>
+    <row r="365" spans="1:5">
+      <c r="A365" s="6"/>
+      <c r="B365" s="6"/>
+      <c r="C365" s="6"/>
+      <c r="D365" s="6"/>
+      <c r="E365" s="6"/>
+    </row>
+    <row r="366" spans="1:5">
+      <c r="A366" s="6"/>
+      <c r="B366" s="6"/>
+      <c r="C366" s="6"/>
+      <c r="D366" s="6"/>
+      <c r="E366" s="6"/>
+    </row>
+    <row r="367" spans="1:5">
+      <c r="A367" s="6"/>
+      <c r="B367" s="6"/>
+      <c r="C367" s="6"/>
+      <c r="D367" s="6"/>
+      <c r="E367" s="6"/>
+    </row>
+    <row r="368" spans="1:5">
+      <c r="A368" s="6"/>
+      <c r="B368" s="6"/>
+      <c r="C368" s="6"/>
+      <c r="D368" s="6"/>
+      <c r="E368" s="6"/>
+    </row>
   </sheetData>
   <sortState ref="A8:J35">
     <sortCondition ref="E8:E35"/>
   </sortState>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>